<commit_message>
modified:   Jack/jack_config.json 	modified:   Jack/jack_test_info.xlsx 	modified:   Zomboni/zomboni_config.json 	modified:   Zomboni/zomboni_test_info.xlsx 	deleted:    output.csv 	new file:   seperate/i1-slow-foot.csv 	new file:   seperate/i1-slow-ladder.csv 	new file:   seperate/i1-slow-pogo.csv 	modified:   seperate/lab.ipynb 	modified:   test.cpp 	deleted:    "\345\210\206\347\246\273\350\256\241\347\256\227/i1-fast-giga.csv" 	deleted:    "\345\210\206\347\246\273\350\256\241\347\256\227/i1-slow-catp.csv" 	deleted:    "\345\210\206\347\246\273\350\256\241\347\256\227/i1-slow-jack.csv" 	deleted:    "\345\210\206\347\246\273\350\256\241\347\256\227/lab.ipynb"
</commit_message>
<xml_diff>
--- a/Jack/jack_test_info.xlsx
+++ b/Jack/jack_test_info.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="12720" windowHeight="3645"/>
+    <workbookView windowWidth="27825" windowHeight="15705"/>
   </bookViews>
   <sheets>
-    <sheet name="6-2" sheetId="1" r:id="rId1"/>
-    <sheet name="6" sheetId="6" r:id="rId2"/>
-    <sheet name="7-N" sheetId="14" r:id="rId3"/>
-    <sheet name="8列炮" sheetId="3" r:id="rId4"/>
+    <sheet name="7-N" sheetId="14" r:id="rId1"/>
+    <sheet name="8列炮" sheetId="3" r:id="rId2"/>
+    <sheet name="6-2" sheetId="1" r:id="rId3"/>
+    <sheet name="6" sheetId="6" r:id="rId4"/>
     <sheet name="奇蛇-N" sheetId="15" r:id="rId5"/>
     <sheet name="5列炮" sheetId="11" r:id="rId6"/>
     <sheet name="5" sheetId="4" r:id="rId7"/>
@@ -39,12 +39,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="46">
   <si>
     <t>小丑类型</t>
   </si>
   <si>
-    <t>早爆</t>
+    <t>全部</t>
   </si>
   <si>
     <t>输出植物信息</t>
@@ -64,7 +64,7 @@
     <t>地图类型</t>
   </si>
   <si>
-    <t>后院</t>
+    <t>前院</t>
   </si>
   <si>
     <t>植物列数</t>
@@ -94,13 +94,10 @@
     <t>曾</t>
   </si>
   <si>
-    <t>非永动</t>
+    <t>永动</t>
   </si>
   <si>
     <t>被炸植物列数</t>
-  </si>
-  <si>
-    <t>永动</t>
   </si>
   <si>
     <t>被炸植物类型</t>
@@ -157,16 +154,10 @@
     <t>灰烬范围(上小下大)</t>
   </si>
   <si>
-    <t>全部</t>
+    <t>早爆</t>
   </si>
   <si>
-    <t>前院</t>
-  </si>
-  <si>
-    <t>上炸下</t>
-  </si>
-  <si>
-    <t>旗帜波</t>
+    <t>后院</t>
   </si>
   <si>
     <t>正炸</t>
@@ -175,7 +166,13 @@
     <t>炮</t>
   </si>
   <si>
-    <t>最快</t>
+    <t>非永动</t>
+  </si>
+  <si>
+    <t>上炸下</t>
+  </si>
+  <si>
+    <t>旗帜波</t>
   </si>
   <si>
     <t>屋顶</t>
@@ -1088,13 +1085,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
-<customStorage xmlns="https://web.wps.cn/et/2018/main">
-  <book/>
-  <sheets/>
-</customStorage>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="WPS">
   <a:themeElements>
@@ -1344,18 +1334,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet13"/>
+  <sheetPr/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
+    <col min="2" max="2" width="10" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.16666666666667" style="1"/>
+    <col min="4" max="4" width="9.33333333333333" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.16666666666667" style="1"/>
+    <col min="7" max="7" width="9.33333333333333" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.16666666666667" style="1"/>
     <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.16666666666667" style="1"/>
     <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
@@ -1365,7 +1359,7 @@
     <col min="15" max="16384" width="9.16666666666667" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:14">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1389,7 +1383,7 @@
       </c>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:14">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1417,7 +1411,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:14">
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1425,7 +1419,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>16</v>
@@ -1434,21 +1428,23 @@
         <v>17</v>
       </c>
       <c r="G3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="3">
-        <v>783</v>
-      </c>
-      <c r="K3" s="3"/>
+        <v>300</v>
+      </c>
+      <c r="K3" s="3">
+        <v>200</v>
+      </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" s="1" customFormat="1" spans="1:14">
+    <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3">
         <v>5</v>
@@ -1457,7 +1453,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -1467,12 +1463,12 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" s="1" customFormat="1" spans="1:14">
+    <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -1481,7 +1477,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -1491,12 +1487,12 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:14">
+    <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -1505,7 +1501,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -1515,15 +1511,15 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" s="1" customFormat="1" spans="4:14">
+    <row r="7" spans="4:14">
       <c r="D7" s="3">
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -1533,9 +1529,9 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="1:14">
+    <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -1544,10 +1540,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -1557,7 +1553,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:14">
+    <row r="9" spans="4:14">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1567,12 +1563,12 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="1:14">
+    <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1583,12 +1579,12 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:14">
+    <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1599,7 +1595,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:14">
+    <row r="12" spans="4:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1609,12 +1605,13 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:14">
+    <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
-        <v>8000</v>
+        <f>B16+299</f>
+        <v>1570</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1625,12 +1622,12 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="1:14">
+    <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
-        <v>3000</v>
+        <v>1400</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1641,12 +1638,12 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="1:14">
+    <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1657,12 +1654,12 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:14">
+    <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3">
-        <v>0</v>
+        <v>1271</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -1673,7 +1670,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" s="1" customFormat="1" spans="4:14">
+    <row r="17" spans="4:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -1683,12 +1680,12 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" s="1" customFormat="1" spans="1:14">
+    <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1699,12 +1696,12 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" s="1" customFormat="1" spans="1:14">
+    <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1715,9 +1712,9 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" s="1" customFormat="1" spans="1:14">
+    <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -1731,10 +1728,10 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" s="1" customFormat="1" spans="1:14">
+    <row r="21" spans="1:14">
       <c r="A21" s="2"/>
       <c r="B21" s="3">
-        <v>100</v>
+        <v>900</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1745,7 +1742,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" s="1" customFormat="1" spans="4:14">
+    <row r="22" spans="4:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1755,9 +1752,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" s="1" customFormat="1" spans="1:14">
-      <c r="A23"/>
-      <c r="B23"/>
+    <row r="23" spans="4:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1767,9 +1762,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:14">
-      <c r="A24"/>
-      <c r="B24"/>
+    <row r="24" spans="4:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1779,7 +1772,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" s="1" customFormat="1" spans="4:14">
+    <row r="25" spans="4:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1866,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1890,7 +1883,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -1927,7 +1920,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -1953,7 +1946,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -1965,10 +1958,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -1977,7 +1970,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -1989,10 +1982,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -2001,7 +1994,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -2016,10 +2009,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2031,7 +2024,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2040,10 +2033,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -2058,10 +2051,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -2073,7 +2066,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -2089,10 +2082,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -2115,7 +2108,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
         <v>549</v>
@@ -2131,7 +2124,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -2147,10 +2140,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2163,7 +2156,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -2189,10 +2182,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -2205,10 +2198,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -2221,7 +2214,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -2365,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2389,7 +2382,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -2426,7 +2419,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -2452,7 +2445,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -2464,10 +2457,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -2476,7 +2469,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -2488,10 +2481,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -2500,7 +2493,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -2515,10 +2508,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2530,7 +2523,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2539,10 +2532,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -2564,7 +2557,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
         <v>100000</v>
@@ -2580,10 +2573,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -2606,7 +2599,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
         <v>8000</v>
@@ -2622,7 +2615,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -2638,10 +2631,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2654,7 +2647,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -2680,10 +2673,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -2696,10 +2689,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -2712,7 +2705,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -2856,7 +2849,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2880,7 +2873,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -2917,7 +2910,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -2943,7 +2936,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -2955,10 +2948,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -2967,7 +2960,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -2979,10 +2972,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -2991,7 +2984,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -3006,10 +2999,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -3021,7 +3014,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -3030,10 +3023,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -3055,7 +3048,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
         <v>500000</v>
@@ -3071,10 +3064,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -3097,7 +3090,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
         <v>2300</v>
@@ -3113,7 +3106,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -3129,10 +3122,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3145,7 +3138,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -3171,10 +3164,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -3187,10 +3180,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -3203,7 +3196,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -3347,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -3371,7 +3364,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -3408,7 +3401,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -3436,7 +3429,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -3448,10 +3441,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -3460,7 +3453,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -3472,10 +3465,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>7</v>
@@ -3484,7 +3477,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -3499,10 +3492,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -3514,7 +3507,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -3523,10 +3516,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -3541,10 +3534,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -3556,7 +3549,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
         <v>50000</v>
@@ -3565,10 +3558,10 @@
         <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
@@ -3580,10 +3573,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -3606,7 +3599,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
         <v>4000</v>
@@ -3622,7 +3615,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -3638,10 +3631,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3654,7 +3647,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -3680,10 +3673,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -3696,10 +3689,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -3712,7 +3705,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -3830,6 +3823,994 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet48"/>
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="1"/>
+    <col min="3" max="8" width="9.16666666666667" style="1"/>
+    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.16666666666667" style="1"/>
+    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.16666666666667" style="1"/>
+    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="3">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="4:14">
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="4:14">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="4:14">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1040</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1400</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="4:14">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3">
+        <v>100</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3">
+        <v>900</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="4:14">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="4:14">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="4:14">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="4:14">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet13"/>
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" style="1"/>
+    <col min="3" max="8" width="9.16666666666667" style="1"/>
+    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.16666666666667" style="1"/>
+    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.16666666666667" style="1"/>
+    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>783</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="4:14">
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="4:14">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:14">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="4:14">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3">
+        <v>8000</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:14">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:14">
+      <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="4:14">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="1:14">
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3">
+        <v>100</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="1:14">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3">
+        <v>100</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="4:14">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="1:14">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="1:14">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="4:14">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N25"/>
@@ -3857,7 +4838,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -3881,7 +4862,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -3909,7 +4890,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -3918,7 +4899,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -3944,7 +4925,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -3956,10 +4937,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -3968,7 +4949,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -3980,10 +4961,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -3992,7 +4973,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -4007,10 +4988,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -4022,7 +5003,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -4031,10 +5012,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -4056,7 +5037,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
         <v>100000000</v>
@@ -4072,10 +5053,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -4098,7 +5079,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
         <v>8000</v>
@@ -4114,7 +5095,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>3000</v>
@@ -4130,10 +5111,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -4146,7 +5127,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -4172,10 +5153,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -4188,10 +5169,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -4204,7 +5185,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -4257,993 +5238,6 @@
     <row r="24" spans="1:14">
       <c r="A24"/>
       <c r="B24"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="4:14">
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:N25"/>
-  <sheetViews>
-    <sheetView zoomScale="221" zoomScaleNormal="221" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.16666666666667" style="1"/>
-    <col min="4" max="4" width="9.33333333333333" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.16666666666667" style="1"/>
-    <col min="7" max="7" width="9.33333333333333" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>300</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="4:14">
-      <c r="D7" s="3">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="4:14">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="4:14">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1570</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1400</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1271</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="4:14">
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="3">
-        <v>100</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3">
-        <v>900</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="4:14">
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="4:14">
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="4:14">
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="4:14">
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet48"/>
-  <dimension ref="A1:N25"/>
-  <sheetViews>
-    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="3">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="4:14">
-      <c r="D7" s="3">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="4:14">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="4:14">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1040</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1400</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="4:14">
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="3">
-        <v>100</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3">
-        <v>900</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="4:14">
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="4:14">
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="4:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -5340,7 +5334,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5364,7 +5358,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -5392,7 +5386,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
@@ -5401,7 +5395,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -5427,7 +5421,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -5439,10 +5433,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -5451,7 +5445,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -5463,10 +5457,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -5475,7 +5469,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -5490,10 +5484,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -5505,7 +5499,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -5514,10 +5508,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -5539,7 +5533,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -5555,10 +5549,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -5581,7 +5575,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
         <v>1116</v>
@@ -5597,7 +5591,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -5613,10 +5607,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -5629,7 +5623,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3">
         <v>696</v>
@@ -5655,10 +5649,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -5671,10 +5665,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -5687,7 +5681,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -5832,7 +5826,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5856,7 +5850,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -5884,7 +5878,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -5893,7 +5887,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -5919,7 +5913,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -5931,10 +5925,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -5943,7 +5937,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -5955,10 +5949,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -5967,7 +5961,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -5982,10 +5976,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -5997,7 +5991,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -6006,10 +6000,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -6024,10 +6018,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -6039,7 +6033,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
         <v>1000000</v>
@@ -6055,10 +6049,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -6081,7 +6075,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
         <v>2301</v>
@@ -6097,7 +6091,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -6113,10 +6107,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -6129,7 +6123,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -6155,10 +6149,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -6171,10 +6165,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -6187,7 +6181,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>0</v>
@@ -6332,7 +6326,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -6356,7 +6350,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -6393,7 +6387,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -6419,7 +6413,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -6431,10 +6425,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -6443,7 +6437,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -6455,10 +6449,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -6467,7 +6461,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -6482,10 +6476,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -6497,7 +6491,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>2</v>
@@ -6506,10 +6500,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -6524,10 +6518,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -6539,7 +6533,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -6555,10 +6549,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -6581,7 +6575,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
         <v>4000</v>
@@ -6597,7 +6591,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -6613,10 +6607,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -6629,7 +6623,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -6655,10 +6649,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -6671,10 +6665,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -6687,7 +6681,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -6832,7 +6826,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -6856,7 +6850,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -6893,7 +6887,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -6919,7 +6913,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -6931,10 +6925,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -6943,7 +6937,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -6955,10 +6949,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -6967,7 +6961,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -6982,10 +6976,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -6997,7 +6991,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -7006,10 +7000,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -7024,10 +7018,10 @@
         <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -7039,7 +7033,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -7055,10 +7049,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -7081,7 +7075,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
         <v>549</v>
@@ -7097,7 +7091,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -7113,10 +7107,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -7129,7 +7123,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -7155,10 +7149,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -7171,10 +7165,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -7187,7 +7181,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -7332,7 +7326,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -7356,7 +7350,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -7393,7 +7387,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -7419,7 +7413,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -7431,10 +7425,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -7443,7 +7437,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -7455,10 +7449,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -7467,7 +7461,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -7482,10 +7476,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -7497,7 +7491,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -7506,10 +7500,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -7524,10 +7518,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -7539,7 +7533,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -7555,10 +7549,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -7581,7 +7575,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
         <v>549</v>
@@ -7597,7 +7591,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -7613,10 +7607,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -7629,7 +7623,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -7655,10 +7649,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -7671,10 +7665,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -7687,7 +7681,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>

</xml_diff>

<commit_message>
modified:   Jack/jack_config.json 	modified:   Jack/jack_test_info.xlsx
</commit_message>
<xml_diff>
--- a/Jack/jack_test_info.xlsx
+++ b/Jack/jack_test_info.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27825" windowHeight="15705"/>
+    <workbookView windowWidth="17190" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet name="7-N" sheetId="14" r:id="rId1"/>
-    <sheet name="8列炮" sheetId="3" r:id="rId2"/>
-    <sheet name="6-2" sheetId="1" r:id="rId3"/>
-    <sheet name="6" sheetId="6" r:id="rId4"/>
+    <sheet name="6" sheetId="6" r:id="rId1"/>
+    <sheet name="7-N" sheetId="14" r:id="rId2"/>
+    <sheet name="8列炮" sheetId="3" r:id="rId3"/>
+    <sheet name="6-2" sheetId="1" r:id="rId4"/>
     <sheet name="奇蛇-N" sheetId="15" r:id="rId5"/>
     <sheet name="5列炮" sheetId="11" r:id="rId6"/>
     <sheet name="5" sheetId="4" r:id="rId7"/>
@@ -64,7 +64,7 @@
     <t>地图类型</t>
   </si>
   <si>
-    <t>前院</t>
+    <t>后院</t>
   </si>
   <si>
     <t>植物列数</t>
@@ -88,16 +88,19 @@
     <t>被炸情况</t>
   </si>
   <si>
-    <t>下炸上</t>
+    <t>上炸下</t>
   </si>
   <si>
     <t>曾</t>
   </si>
   <si>
-    <t>永动</t>
+    <t>非永动</t>
   </si>
   <si>
     <t>被炸植物列数</t>
+  </si>
+  <si>
+    <t>永动</t>
   </si>
   <si>
     <t>被炸植物类型</t>
@@ -136,7 +139,7 @@
     <t>灰烬类型</t>
   </si>
   <si>
-    <t>卡</t>
+    <t>炮</t>
   </si>
   <si>
     <t>植物可伤时机</t>
@@ -154,28 +157,25 @@
     <t>灰烬范围(上小下大)</t>
   </si>
   <si>
-    <t>早爆</t>
+    <t>前院</t>
   </si>
   <si>
-    <t>后院</t>
+    <t>下炸上</t>
+  </si>
+  <si>
+    <t>卡</t>
+  </si>
+  <si>
+    <t>早爆</t>
   </si>
   <si>
     <t>正炸</t>
   </si>
   <si>
-    <t>炮</t>
-  </si>
-  <si>
-    <t>非永动</t>
-  </si>
-  <si>
-    <t>上炸下</t>
+    <t>屋顶</t>
   </si>
   <si>
     <t>旗帜波</t>
-  </si>
-  <si>
-    <t>屋顶</t>
   </si>
   <si>
     <t>最慢</t>
@@ -1334,22 +1334,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.16666666666667" style="1"/>
-    <col min="4" max="4" width="9.33333333333333" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.16666666666667" style="1"/>
-    <col min="7" max="7" width="9.33333333333333" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.16666666666667" style="1"/>
+    <col min="2" max="2" width="10.375" style="1"/>
+    <col min="3" max="8" width="9.16666666666667" style="1"/>
     <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.16666666666667" style="1"/>
     <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
@@ -1419,7 +1415,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>16</v>
@@ -1428,14 +1424,12 @@
         <v>17</v>
       </c>
       <c r="G3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="3">
-        <v>300</v>
-      </c>
-      <c r="K3" s="3">
-        <v>200</v>
-      </c>
+        <v>395</v>
+      </c>
+      <c r="K3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
@@ -1444,7 +1438,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3">
         <v>5</v>
@@ -1453,7 +1447,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -1465,10 +1459,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -1477,7 +1471,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -1489,10 +1483,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -1501,7 +1495,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -1516,10 +1510,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -1531,7 +1525,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -1540,10 +1534,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -1565,7 +1559,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -1581,10 +1575,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1607,11 +1601,10 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
-        <f>B16+299</f>
-        <v>1570</v>
+        <v>1928</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1624,10 +1617,10 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
-        <v>1400</v>
+        <v>3000</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1640,10 +1633,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1656,10 +1649,10 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
-        <v>1271</v>
+        <v>0</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -1682,10 +1675,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1698,10 +1691,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1714,7 +1707,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -1752,7 +1745,9 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14">
+    <row r="23" spans="1:14">
+      <c r="A23"/>
+      <c r="B23"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1762,7 +1757,9 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14">
+    <row r="24" spans="1:14">
+      <c r="A24"/>
+      <c r="B24"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1859,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1883,7 +1880,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -1911,7 +1908,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>9</v>
@@ -1920,7 +1917,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -1946,7 +1943,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -1958,10 +1955,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -1970,7 +1967,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -1982,10 +1979,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -1994,7 +1991,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -2009,10 +2006,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2024,7 +2021,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2033,10 +2030,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -2051,10 +2048,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -2066,7 +2063,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -2082,10 +2079,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -2108,7 +2105,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
         <v>549</v>
@@ -2124,7 +2121,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -2140,10 +2137,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2156,7 +2153,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -2182,7 +2179,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>45</v>
@@ -2198,10 +2195,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -2214,7 +2211,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -2382,7 +2379,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -2410,7 +2407,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -2419,7 +2416,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -2445,7 +2442,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -2457,10 +2454,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -2469,7 +2466,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -2481,10 +2478,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -2493,7 +2490,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -2508,10 +2505,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2523,7 +2520,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2532,10 +2529,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -2557,7 +2554,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>100000</v>
@@ -2573,10 +2570,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -2599,7 +2596,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
         <v>8000</v>
@@ -2615,7 +2612,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -2631,10 +2628,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2647,7 +2644,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -2673,10 +2670,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -2689,10 +2686,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -2705,7 +2702,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -2873,7 +2870,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -2901,7 +2898,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -2910,7 +2907,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -2936,7 +2933,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -2948,10 +2945,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -2960,7 +2957,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -2972,10 +2969,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -2984,7 +2981,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -2999,10 +2996,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -3014,7 +3011,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -3023,10 +3020,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -3048,7 +3045,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>500000</v>
@@ -3064,10 +3061,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -3090,7 +3087,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
         <v>2300</v>
@@ -3106,7 +3103,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -3122,10 +3119,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3138,7 +3135,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -3164,10 +3161,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -3180,10 +3177,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -3196,7 +3193,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -3340,7 +3337,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -3364,7 +3361,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -3392,7 +3389,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>5</v>
@@ -3401,7 +3398,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -3429,7 +3426,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -3441,10 +3438,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -3453,7 +3450,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -3465,10 +3462,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>7</v>
@@ -3477,7 +3474,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -3492,10 +3489,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -3507,7 +3504,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -3516,10 +3513,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -3534,10 +3531,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -3549,7 +3546,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>50000</v>
@@ -3558,10 +3555,10 @@
         <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
@@ -3573,10 +3570,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -3599,7 +3596,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
         <v>4000</v>
@@ -3615,7 +3612,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -3631,10 +3628,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3647,7 +3644,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -3673,10 +3670,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -3689,10 +3686,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -3705,7 +3702,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -3823,6 +3820,505 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.16666666666667" style="1"/>
+    <col min="4" max="4" width="9.33333333333333" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.16666666666667" style="1"/>
+    <col min="7" max="7" width="9.33333333333333" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.16666666666667" style="1"/>
+    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.16666666666667" style="1"/>
+    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.16666666666667" style="1"/>
+    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="3">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>300</v>
+      </c>
+      <c r="K3" s="3">
+        <v>200</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="4:14">
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="4:14">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="4:14">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3">
+        <f>B16+299</f>
+        <v>1570</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1400</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1271</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="4:14">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3">
+        <v>100</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3">
+        <v>900</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="4:14">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="4:14">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="4:14">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="4:14">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet48"/>
   <dimension ref="A1:N25"/>
@@ -3850,7 +4346,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -3874,7 +4370,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -3902,7 +4398,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
@@ -3911,7 +4407,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -3937,7 +4433,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -3949,10 +4445,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -3961,7 +4457,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -3973,10 +4469,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -3985,7 +4481,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -4000,10 +4496,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -4015,7 +4511,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -4024,10 +4520,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -4049,7 +4545,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -4065,10 +4561,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -4091,7 +4587,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
         <v>1040</v>
@@ -4107,7 +4603,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -4123,10 +4619,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -4139,7 +4635,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -4165,10 +4661,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -4181,10 +4677,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -4197,7 +4693,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -4314,7 +4810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:N25"/>
@@ -4342,7 +4838,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -4366,7 +4862,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -4394,7 +4890,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -4403,7 +4899,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -4429,7 +4925,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -4441,10 +4937,10 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -4453,7 +4949,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -4465,10 +4961,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -4477,7 +4973,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -4492,10 +4988,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -4507,7 +5003,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -4516,10 +5012,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -4541,7 +5037,7 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>100000000</v>
@@ -4557,10 +5053,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -4583,7 +5079,7 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
         <v>8000</v>
@@ -4599,7 +5095,7 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>3000</v>
@@ -4615,10 +5111,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -4631,7 +5127,7 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -4657,10 +5153,10 @@
     </row>
     <row r="18" s="1" customFormat="1" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -4673,10 +5169,10 @@
     </row>
     <row r="19" s="1" customFormat="1" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -4689,7 +5185,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -4752,502 +5248,6 @@
       <c r="N24" s="2"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="4:14">
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:N25"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="3">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>901</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="4:14">
-      <c r="D7" s="3">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="4:14">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3">
-        <v>100000000</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="4:14">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3">
-        <v>8000</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2">
-        <v>3000</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="4:14">
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="3">
-        <v>100</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3">
-        <v>100</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="4:14">
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="4:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -5334,7 +5334,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5358,7 +5358,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -5386,7 +5386,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
@@ -5395,7 +5395,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -5421,7 +5421,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -5433,10 +5433,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -5445,7 +5445,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -5457,10 +5457,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -5469,7 +5469,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -5484,10 +5484,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -5499,7 +5499,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -5508,10 +5508,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -5533,7 +5533,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -5549,10 +5549,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -5575,7 +5575,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
         <v>1116</v>
@@ -5591,7 +5591,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -5607,10 +5607,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -5623,7 +5623,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>696</v>
@@ -5649,10 +5649,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -5665,10 +5665,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -5681,7 +5681,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -5800,7 +5800,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
@@ -5850,7 +5850,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -5878,7 +5878,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -5887,7 +5887,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -5913,7 +5913,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -5925,10 +5925,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -5937,7 +5937,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -5949,10 +5949,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -5961,7 +5961,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -5976,10 +5976,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -5991,7 +5991,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -6000,10 +6000,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -6018,10 +6018,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -6033,7 +6033,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>1000000</v>
@@ -6049,10 +6049,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -6075,7 +6075,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
         <v>2301</v>
@@ -6091,7 +6091,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -6107,10 +6107,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -6123,7 +6123,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -6149,10 +6149,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -6165,10 +6165,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -6181,7 +6181,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>0</v>
@@ -6300,7 +6300,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
@@ -6350,7 +6350,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -6378,7 +6378,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -6387,7 +6387,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -6413,7 +6413,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -6425,10 +6425,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -6437,7 +6437,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -6449,10 +6449,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -6461,7 +6461,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -6476,10 +6476,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -6491,7 +6491,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>2</v>
@@ -6500,10 +6500,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -6518,10 +6518,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -6533,7 +6533,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -6549,10 +6549,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -6575,7 +6575,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
         <v>4000</v>
@@ -6591,7 +6591,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -6607,10 +6607,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -6623,7 +6623,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -6649,10 +6649,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -6665,10 +6665,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -6681,7 +6681,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -6850,7 +6850,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -6878,7 +6878,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>9</v>
@@ -6887,7 +6887,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -6913,7 +6913,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -6925,10 +6925,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -6937,7 +6937,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -6949,10 +6949,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -6961,7 +6961,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -6976,10 +6976,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -6991,7 +6991,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -7000,10 +7000,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -7018,10 +7018,10 @@
         <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -7033,7 +7033,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -7049,10 +7049,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -7075,7 +7075,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
         <v>549</v>
@@ -7091,7 +7091,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -7107,10 +7107,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -7123,7 +7123,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -7149,10 +7149,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -7165,10 +7165,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -7181,7 +7181,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -7326,7 +7326,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -7350,7 +7350,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -7378,7 +7378,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3">
         <v>9</v>
@@ -7387,7 +7387,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -7413,7 +7413,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -7425,10 +7425,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -7437,7 +7437,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -7449,10 +7449,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -7461,7 +7461,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -7476,10 +7476,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -7491,7 +7491,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -7500,10 +7500,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -7518,10 +7518,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -7533,7 +7533,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -7549,10 +7549,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -7575,7 +7575,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
         <v>549</v>
@@ -7591,7 +7591,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>4000</v>
@@ -7607,10 +7607,10 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -7623,7 +7623,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -7649,7 +7649,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>45</v>
@@ -7665,10 +7665,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -7681,7 +7681,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>

</xml_diff>

<commit_message>
modified:   Jack/jack_config.json 	modified:   Jack/jack_test_info.xlsx 	modified:   Zomboni/Zomboni_cpp_1_0.cpp 	modified:   Zomboni/zomboni_config.json 	modified:   Zomboni/zomboni_test_info.xlsx 	Jack/Jack_cpp_1_0.exe 	Jack/batch_test/Jack_cpp_1_0.exe 	Zomboni/Zomboni_cpp_1_0.exe 	Zomboni/~$zomboni_test_info.xlsx
</commit_message>
<xml_diff>
--- a/Jack/jack_test_info.xlsx
+++ b/Jack/jack_test_info.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="17400" windowHeight="11490"/>
+    <workbookView windowWidth="16005" windowHeight="14025"/>
   </bookViews>
   <sheets>
     <sheet name="6" sheetId="6" r:id="rId1"/>
-    <sheet name="7-N" sheetId="14" r:id="rId2"/>
-    <sheet name="8列炮" sheetId="3" r:id="rId3"/>
-    <sheet name="6-2" sheetId="1" r:id="rId4"/>
-    <sheet name="奇蛇-N" sheetId="15" r:id="rId5"/>
-    <sheet name="5列炮" sheetId="11" r:id="rId6"/>
-    <sheet name="5" sheetId="4" r:id="rId7"/>
-    <sheet name="7" sheetId="13" r:id="rId8"/>
-    <sheet name="9-2" sheetId="12" r:id="rId9"/>
-    <sheet name="9" sheetId="5" r:id="rId10"/>
-    <sheet name="3" sheetId="10" r:id="rId11"/>
+    <sheet name="3" sheetId="10" r:id="rId2"/>
+    <sheet name="7-N" sheetId="14" r:id="rId3"/>
+    <sheet name="8列炮" sheetId="3" r:id="rId4"/>
+    <sheet name="6-2" sheetId="1" r:id="rId5"/>
+    <sheet name="奇蛇-N" sheetId="15" r:id="rId6"/>
+    <sheet name="5列炮" sheetId="11" r:id="rId7"/>
+    <sheet name="5" sheetId="4" r:id="rId8"/>
+    <sheet name="7" sheetId="13" r:id="rId9"/>
+    <sheet name="9-2" sheetId="12" r:id="rId10"/>
+    <sheet name="9" sheetId="5" r:id="rId11"/>
     <sheet name="4" sheetId="9" r:id="rId12"/>
     <sheet name="8" sheetId="8" r:id="rId13"/>
   </sheets>
@@ -39,12 +39,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="46">
   <si>
     <t>小丑类型</t>
   </si>
   <si>
-    <t>全部</t>
+    <t>早爆</t>
   </si>
   <si>
     <t>输出植物信息</t>
@@ -88,7 +88,7 @@
     <t>被炸情况</t>
   </si>
   <si>
-    <t>上炸下</t>
+    <t>正炸</t>
   </si>
   <si>
     <t>曾</t>
@@ -103,7 +103,7 @@
     <t>被炸植物类型</t>
   </si>
   <si>
-    <t>南瓜</t>
+    <t>普通</t>
   </si>
   <si>
     <t>波次类型</t>
@@ -154,25 +154,22 @@
     <t>灰烬范围(上小下大)</t>
   </si>
   <si>
+    <t>全部</t>
+  </si>
+  <si>
     <t>前院</t>
   </si>
   <si>
-    <t>下炸上</t>
+    <t>上炸下</t>
   </si>
   <si>
-    <t>普通</t>
+    <t>非永动</t>
   </si>
   <si>
     <t>卡</t>
   </si>
   <si>
-    <t>早爆</t>
-  </si>
-  <si>
-    <t>正炸</t>
-  </si>
-  <si>
-    <t>非永动</t>
+    <t>下炸上</t>
   </si>
   <si>
     <t>屋顶</t>
@@ -1341,7 +1338,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
@@ -1832,6 +1829,506 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView zoomScale="116" zoomScaleNormal="116" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33333333333333" style="1"/>
+    <col min="3" max="8" width="9.16666666666667" style="1"/>
+    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.16666666666667" style="1"/>
+    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.16666666666667" style="1"/>
+    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="3">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="K3" s="3">
+        <v>307</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="4:14">
+      <c r="D7" s="3">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="4:14">
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="4:14">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3">
+        <v>549</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4000</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="4:14">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3">
+        <v>100</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3">
+        <v>716</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="4:14">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="4:14">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="4:14">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="4:14">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N25"/>
@@ -1859,7 +2356,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1911,7 +2408,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <v>9</v>
@@ -1920,7 +2417,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -1946,7 +2443,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -1961,7 +2458,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -1970,7 +2467,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -1985,7 +2482,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -2012,7 +2509,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2185,7 +2682,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -2232,497 +2729,6 @@
       <c r="A21" s="2"/>
       <c r="B21" s="3">
         <v>716</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="4:14">
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="4:14">
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="4:14">
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="4:14">
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:N25"/>
-  <sheetViews>
-    <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="3">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>300</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="4:14">
-      <c r="D7" s="3">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>3</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="4:14">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3">
-        <v>100000</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="4:14">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3">
-        <v>8000</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2">
-        <v>4000</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="4:14">
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="3">
-        <v>100</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3">
-        <v>100</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -2849,7 +2855,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2901,7 +2907,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -2910,7 +2916,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -2951,7 +2957,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -3125,7 +3131,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3340,7 +3346,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -3392,7 +3398,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <v>5</v>
@@ -3444,7 +3450,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -3634,7 +3640,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3823,6 +3829,501 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="1"/>
+    <col min="3" max="8" width="9.16666666666667" style="1"/>
+    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.16666666666667" style="1"/>
+    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.16666666666667" style="1"/>
+    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>830</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <f>I3+2501</f>
+        <v>3331</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="4:14">
+      <c r="D7" s="3">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="4:14">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="4:14">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3">
+        <v>8000</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4000</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="4:14">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3">
+        <v>-200</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="4:14">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="4:14">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="4:14">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="4:14">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N25"/>
@@ -3854,7 +4355,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -3878,7 +4379,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -3906,7 +4407,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
@@ -3958,7 +4459,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -4133,7 +4634,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -4321,7 +4822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet48"/>
   <dimension ref="A1:N25"/>
@@ -4349,7 +4850,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -4401,7 +4902,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
@@ -4813,7 +5314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:N25"/>
@@ -4841,7 +5342,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -4893,7 +5394,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -4902,7 +5403,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -4943,7 +5444,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -5117,7 +5618,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -5309,7 +5810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N25"/>
@@ -5337,7 +5838,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5361,7 +5862,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -5389,7 +5890,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
@@ -5439,7 +5940,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -5613,7 +6114,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -5801,7 +6302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:N25"/>
@@ -5829,7 +6330,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5881,7 +6382,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -6301,7 +6802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:N25"/>
@@ -6329,7 +6830,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -6381,7 +6882,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -6431,7 +6932,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -6613,7 +7114,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -6801,7 +7302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N25"/>
@@ -6829,7 +7330,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -6881,7 +7382,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <v>9</v>
@@ -6890,7 +7391,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -6931,7 +7432,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -6982,7 +7483,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -7299,504 +7800,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:N25"/>
-  <sheetViews>
-    <sheetView zoomScale="116" zoomScaleNormal="116" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33333333333333" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="3">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="K3" s="3">
-        <v>307</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="3">
-        <v>7</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="3">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="4:14">
-      <c r="D7" s="3">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>6</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="4:14">
-      <c r="D9" s="3">
-        <v>5</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="4:14">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3">
-        <v>549</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2">
-        <v>4000</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="4:14">
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="3">
-        <v>100</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3">
-        <v>716</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="4:14">
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="4:14">
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="4:14">
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="4:14">
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
modified:   Jack/jack_config.json 	modified:   Jack/jack_test_info.xlsx 	modified:   output.csv 	modified:   test.cpp 	modified:   "\347\275\256\344\277\241\345\214\272\351\227\264\344\270\216\345\201\207\350\256\276\346\243\200\351\252\214.ipynb"
</commit_message>
<xml_diff>
--- a/Jack/jack_test_info.xlsx
+++ b/Jack/jack_test_info.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="16005" windowHeight="14025"/>
+    <workbookView windowWidth="15720" windowHeight="9750"/>
   </bookViews>
   <sheets>
-    <sheet name="6" sheetId="6" r:id="rId1"/>
-    <sheet name="3" sheetId="10" r:id="rId2"/>
-    <sheet name="7-N" sheetId="14" r:id="rId3"/>
-    <sheet name="8列炮" sheetId="3" r:id="rId4"/>
-    <sheet name="6-2" sheetId="1" r:id="rId5"/>
-    <sheet name="奇蛇-N" sheetId="15" r:id="rId6"/>
-    <sheet name="5列炮" sheetId="11" r:id="rId7"/>
-    <sheet name="5" sheetId="4" r:id="rId8"/>
+    <sheet name="8列炮" sheetId="3" r:id="rId1"/>
+    <sheet name="5" sheetId="4" r:id="rId2"/>
+    <sheet name="6" sheetId="6" r:id="rId3"/>
+    <sheet name="3" sheetId="10" r:id="rId4"/>
+    <sheet name="7-N" sheetId="14" r:id="rId5"/>
+    <sheet name="6-2" sheetId="1" r:id="rId6"/>
+    <sheet name="奇蛇-N" sheetId="15" r:id="rId7"/>
+    <sheet name="5列炮" sheetId="11" r:id="rId8"/>
     <sheet name="7" sheetId="13" r:id="rId9"/>
     <sheet name="9-2" sheetId="12" r:id="rId10"/>
     <sheet name="9" sheetId="5" r:id="rId11"/>
@@ -44,7 +44,7 @@
     <t>小丑类型</t>
   </si>
   <si>
-    <t>早爆</t>
+    <t>全部</t>
   </si>
   <si>
     <t>输出植物信息</t>
@@ -103,13 +103,13 @@
     <t>被炸植物类型</t>
   </si>
   <si>
-    <t>普通</t>
+    <t>炮</t>
   </si>
   <si>
     <t>波次类型</t>
   </si>
   <si>
-    <t>通常波</t>
+    <t>旗帜波</t>
   </si>
   <si>
     <t>喷</t>
@@ -136,9 +136,6 @@
     <t>灰烬类型</t>
   </si>
   <si>
-    <t>炮</t>
-  </si>
-  <si>
     <t>植物可伤时机</t>
   </si>
   <si>
@@ -154,7 +151,22 @@
     <t>灰烬范围(上小下大)</t>
   </si>
   <si>
-    <t>全部</t>
+    <t>下炸上</t>
+  </si>
+  <si>
+    <t>非永动</t>
+  </si>
+  <si>
+    <t>普通</t>
+  </si>
+  <si>
+    <t>卡</t>
+  </si>
+  <si>
+    <t>早爆</t>
+  </si>
+  <si>
+    <t>通常波</t>
   </si>
   <si>
     <t>前院</t>
@@ -163,19 +175,7 @@
     <t>上炸下</t>
   </si>
   <si>
-    <t>非永动</t>
-  </si>
-  <si>
-    <t>卡</t>
-  </si>
-  <si>
-    <t>下炸上</t>
-  </si>
-  <si>
     <t>屋顶</t>
-  </si>
-  <si>
-    <t>旗帜波</t>
   </si>
   <si>
     <t>最慢</t>
@@ -1334,17 +1334,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet5"/>
+  <sheetPr codeName="Sheet48"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1"/>
+    <col min="2" max="2" width="9.375" style="1"/>
     <col min="3" max="8" width="9.16666666666667" style="1"/>
     <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.16666666666667" style="1"/>
@@ -1415,7 +1415,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>16</v>
@@ -1424,10 +1424,10 @@
         <v>17</v>
       </c>
       <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
         <v>1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>783</v>
       </c>
       <c r="K3" s="3"/>
       <c r="M3" s="2"/>
@@ -1438,7 +1438,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3">
         <v>5</v>
@@ -1450,7 +1450,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3"/>
       <c r="K4" s="3"/>
@@ -1604,7 +1604,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="3">
-        <v>1928</v>
+        <v>1831</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1620,7 +1620,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="2">
-        <v>3000</v>
+        <v>1400</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1636,7 +1636,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -1675,10 +1675,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1691,10 +1691,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -1745,9 +1745,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14">
-      <c r="A23"/>
-      <c r="B23"/>
+    <row r="23" spans="4:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1757,9 +1755,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14">
-      <c r="A24"/>
-      <c r="B24"/>
+    <row r="24" spans="4:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1856,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1908,7 +1904,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3">
         <v>9</v>
@@ -1917,7 +1913,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -1943,7 +1939,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -1958,7 +1954,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -1967,7 +1963,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -1982,7 +1978,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -2009,7 +2005,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2140,7 +2136,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2153,7 +2149,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -2179,7 +2175,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>45</v>
@@ -2195,10 +2191,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -2211,7 +2207,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -2356,7 +2352,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2408,7 +2404,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3">
         <v>9</v>
@@ -2417,7 +2413,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -2443,7 +2439,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -2458,7 +2454,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -2467,7 +2463,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -2482,7 +2478,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -2509,7 +2505,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2640,7 +2636,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2653,7 +2649,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -2679,7 +2675,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>45</v>
@@ -2695,10 +2691,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -2711,7 +2707,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -2855,7 +2851,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2907,7 +2903,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -2916,7 +2912,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -2957,7 +2953,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -2981,7 +2977,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -3131,7 +3127,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3144,7 +3140,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -3170,10 +3166,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -3186,10 +3182,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -3202,7 +3198,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -3346,7 +3342,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -3398,7 +3394,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3">
         <v>5</v>
@@ -3450,7 +3446,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -3474,7 +3470,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3">
         <v>7</v>
@@ -3640,7 +3636,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3653,7 +3649,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -3679,10 +3675,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -3695,10 +3691,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -3711,7 +3707,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -3829,6 +3825,1002 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet25"/>
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33333333333333" style="1"/>
+    <col min="3" max="8" width="9.16666666666667" style="1"/>
+    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.16666666666667" style="1"/>
+    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.16666666666667" style="1"/>
+    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>901</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="4:14">
+      <c r="D7" s="3">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="4:14">
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="4:14">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3">
+        <v>4000</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4000</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="4:14">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="3">
+        <v>100</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3">
+        <v>100</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="4:14">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="4:14">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="4:14">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="4:14">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" style="1"/>
+    <col min="3" max="8" width="9.16666666666667" style="1"/>
+    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.16666666666667" style="1"/>
+    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.16666666666667" style="1"/>
+    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>783</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="4:14">
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="4:14">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="4:14">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1928</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="4:14">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="3">
+        <v>100</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3">
+        <v>900</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="4:14">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="4:14">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:N25"/>
@@ -3856,7 +4848,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -3880,7 +4872,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -3908,7 +4900,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -3917,7 +4909,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -3961,7 +4953,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -3985,7 +4977,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -4135,7 +5127,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -4148,7 +5140,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -4174,10 +5166,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -4190,10 +5182,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -4206,7 +5198,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>-200</v>
@@ -4323,7 +5315,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N25"/>
@@ -4355,7 +5347,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -4379,7 +5371,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -4407,7 +5399,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
@@ -4459,7 +5451,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -4483,7 +5475,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -4634,7 +5626,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -4647,7 +5639,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>1271</v>
@@ -4673,10 +5665,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -4689,10 +5681,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -4705,7 +5697,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -4822,499 +5814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet48"/>
-  <dimension ref="A1:N25"/>
-  <sheetViews>
-    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="4:14">
-      <c r="D7" s="3">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="4:14">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="4:14">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1040</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1400</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="4:14">
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="3">
-        <v>100</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3">
-        <v>900</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="4:14">
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="4:14">
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="4:14">
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="4:14">
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:N25"/>
@@ -5342,7 +5842,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5394,7 +5894,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -5403,7 +5903,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -5444,7 +5944,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -5468,7 +5968,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -5618,7 +6118,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -5631,7 +6131,7 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -5657,10 +6157,10 @@
     </row>
     <row r="18" s="1" customFormat="1" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -5673,10 +6173,10 @@
     </row>
     <row r="19" s="1" customFormat="1" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -5689,7 +6189,7 @@
     </row>
     <row r="20" s="1" customFormat="1" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -5810,7 +6310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N25"/>
@@ -5838,7 +6338,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5862,7 +6362,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -5940,7 +6440,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -5964,7 +6464,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -6114,7 +6614,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -6127,7 +6627,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>696</v>
@@ -6153,10 +6653,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -6169,10 +6669,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -6185,7 +6685,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -6302,7 +6802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:N25"/>
@@ -6330,7 +6830,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -6432,7 +6932,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -6456,7 +6956,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -6614,7 +7114,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -6627,7 +7127,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -6653,10 +7153,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -6669,10 +7169,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -6685,7 +7185,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>0</v>
@@ -6703,506 +7203,6 @@
       <c r="A21" s="2"/>
       <c r="B21" s="3">
         <v>1000</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="4:14">
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="4:14">
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="4:14">
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="4:14">
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet25"/>
-  <dimension ref="A1:N25"/>
-  <sheetViews>
-    <sheetView zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33333333333333" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="3">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>300</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="4:14">
-      <c r="D7" s="3">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3">
-        <v>3</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="4:14">
-      <c r="D9" s="3">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="4:14">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3">
-        <v>4000</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2">
-        <v>4000</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-    </row>
-    <row r="17" spans="4:14">
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="3">
-        <v>100</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3">
-        <v>100</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -7330,7 +7330,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -7382,7 +7382,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3">
         <v>9</v>
@@ -7391,7 +7391,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -7432,7 +7432,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -7456,7 +7456,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -7483,7 +7483,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -7614,7 +7614,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -7627,7 +7627,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -7653,10 +7653,10 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -7669,10 +7669,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -7685,7 +7685,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>

</xml_diff>

<commit_message>
modified:   Jack/jack_config.json 	modified:   Jack/jack_test_info.xlsx 	modified:   output.csv 	modified:   test.cpp
</commit_message>
<xml_diff>
--- a/Jack/jack_test_info.xlsx
+++ b/Jack/jack_test_info.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11116"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qiaoli/Desktop/THU/simu_cpp/Jack/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096051CC-DFBC-DF4C-817E-C242F18C7DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="15720" windowHeight="9750"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15720" windowHeight="9760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="8列炮" sheetId="3" r:id="rId1"/>
@@ -30,7 +36,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="47">
   <si>
     <t>小丑类型</t>
   </si>
@@ -180,18 +185,15 @@
   <si>
     <t>最慢</t>
   </si>
+  <si>
+    <t>最快</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,151 +202,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,192 +218,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -546,255 +237,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -808,92 +257,164 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <color theme="1"/>
       </font>
       <border>
@@ -904,7 +425,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <color theme="0"/>
       </font>
       <fill>
@@ -932,154 +453,40 @@
           <color theme="4"/>
         </bottom>
         <horizontal style="thin">
-          <color theme="4" tint="0.399975585192419"/>
+          <color theme="4" tint="0.39994506668294322"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="firstColumn" dxfId="13"/>
+      <tableStyleElement type="lastColumn" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
-      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="totalRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="5"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="4"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="3"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="2"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="1"/>
+      <tableStyleElement type="pageFieldValues" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1329,30 +736,35 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet48"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1"/>
+    <col min="7" max="7" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1360,24 +772,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -1398,8 +810,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1427,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="3">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="K3" s="3"/>
       <c r="M3" s="2"/>
@@ -1486,7 +898,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -1505,7 +917,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>5</v>
       </c>
@@ -1547,7 +959,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1589,7 +1001,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1604,7 +1016,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="3">
-        <v>1831</v>
+        <v>938</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1663,7 +1075,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -1678,7 +1090,7 @@
         <v>32</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1706,7 +1118,7 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -1722,7 +1134,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>900</v>
       </c>
@@ -1735,7 +1147,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1745,7 +1157,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14">
+    <row r="23" spans="1:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1755,7 +1167,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14">
+    <row r="24" spans="1:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1765,7 +1177,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1783,68 +1195,68 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView zoomScale="116" zoomScaleNormal="116" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33333333333333" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1"/>
+    <col min="3" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1854,22 +1266,22 @@
       <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -1890,8 +1302,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1997,7 +1409,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>7</v>
       </c>
@@ -2039,7 +1451,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3">
         <v>5</v>
       </c>
@@ -2089,7 +1501,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -2163,7 +1575,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -2206,7 +1618,7 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -2222,7 +1634,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>716</v>
       </c>
@@ -2235,7 +1647,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -2245,7 +1657,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14">
+    <row r="23" spans="1:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -2255,7 +1667,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14">
+    <row r="24" spans="1:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -2265,7 +1677,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -2283,49 +1695,49 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0900-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0900-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0900-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0900-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0900-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0900-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0900-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0900-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0900-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0900-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0900-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
@@ -2333,18 +1745,18 @@
       <selection activeCell="A19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33333333333333" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1"/>
+    <col min="3" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2354,22 +1766,22 @@
       <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -2390,8 +1802,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2497,7 +1909,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>7</v>
       </c>
@@ -2539,7 +1951,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3">
         <v>5</v>
       </c>
@@ -2589,7 +2001,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -2663,7 +2075,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -2706,7 +2118,7 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -2722,7 +2134,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>716</v>
       </c>
@@ -2735,7 +2147,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -2745,7 +2157,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14">
+    <row r="23" spans="1:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -2755,7 +2167,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14">
+    <row r="24" spans="1:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -2765,7 +2177,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -2783,67 +2195,67 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0A00-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0A00-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0A00-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0A00-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0A00-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0A00-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0A00-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0A00-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0A00-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0A00-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0A00-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet34"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView zoomScale="117" zoomScaleNormal="117" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2853,22 +2265,22 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -2889,8 +2301,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2996,7 +2408,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>4</v>
       </c>
@@ -3038,7 +2450,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -3080,7 +2492,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -3154,7 +2566,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -3197,7 +2609,7 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -3213,7 +2625,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>100</v>
       </c>
@@ -3226,7 +2638,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -3236,7 +2648,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14">
+    <row r="23" spans="1:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -3246,7 +2658,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14">
+    <row r="24" spans="1:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -3256,7 +2668,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -3274,67 +2686,67 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0B00-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0B00-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0B00-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0B00-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0B00-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0B00-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0B00-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0B00-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0B00-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0B00-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0B00-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView zoomScale="117" zoomScaleNormal="117" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -3344,22 +2756,22 @@
       <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -3380,8 +2792,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3489,7 +2901,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>7</v>
       </c>
@@ -3531,7 +2943,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3">
         <v>5</v>
       </c>
@@ -3589,7 +3001,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -3663,7 +3075,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -3706,7 +3118,7 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -3722,7 +3134,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>100</v>
       </c>
@@ -3735,7 +3147,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -3745,7 +3157,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14">
+    <row r="23" spans="1:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -3755,7 +3167,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14">
+    <row r="24" spans="1:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -3765,7 +3177,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -3783,49 +3195,49 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0C00-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0C00-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0C00-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0C00-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0C00-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0C00-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0C00-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0C00-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0C00-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0C00-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0C00-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
@@ -3833,18 +3245,18 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33333333333333" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1"/>
+    <col min="3" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -3854,22 +3266,22 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -3890,8 +3302,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3997,7 +3409,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>4</v>
       </c>
@@ -4039,7 +3451,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3">
         <v>2</v>
       </c>
@@ -4089,7 +3501,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -4163,7 +3575,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -4206,7 +3618,7 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -4222,7 +3634,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>100</v>
       </c>
@@ -4235,7 +3647,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -4245,7 +3657,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14">
+    <row r="23" spans="1:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -4255,7 +3667,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14">
+    <row r="24" spans="1:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -4265,7 +3677,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -4283,49 +3695,49 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0100-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0100-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0100-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0100-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0100-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0100-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
@@ -4333,18 +3745,18 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1"/>
+    <col min="3" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -4354,22 +3766,22 @@
       <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -4390,8 +3802,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -4497,7 +3909,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>5</v>
       </c>
@@ -4539,7 +3951,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -4581,7 +3993,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -4655,7 +4067,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -4698,7 +4110,7 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -4714,7 +4126,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>900</v>
       </c>
@@ -4727,7 +4139,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -4761,7 +4173,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -4779,49 +4191,49 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0200-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0200-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0200-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0200-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0200-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0200-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
@@ -4829,18 +4241,18 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1"/>
+    <col min="3" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -4850,22 +4262,22 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -4886,8 +4298,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -4996,7 +4408,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>4</v>
       </c>
@@ -5038,7 +4450,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -5080,7 +4492,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -5154,7 +4566,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -5197,7 +4609,7 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -5213,7 +4625,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>1000</v>
       </c>
@@ -5226,7 +4638,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -5236,7 +4648,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14">
+    <row r="23" spans="1:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -5246,7 +4658,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14">
+    <row r="24" spans="1:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -5256,7 +4668,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -5274,49 +4686,49 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0300-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0300-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0300-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0300-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0300-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0300-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0300-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0300-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0300-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0300-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
@@ -5324,22 +4736,22 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.16666666666667" style="1"/>
-    <col min="4" max="4" width="9.33333333333333" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.16666666666667" style="1"/>
-    <col min="7" max="7" width="9.33333333333333" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1"/>
+    <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -5349,22 +4761,22 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -5385,8 +4797,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -5494,7 +4906,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>5</v>
       </c>
@@ -5536,7 +4948,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -5578,7 +4990,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -5653,7 +5065,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -5696,7 +5108,7 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -5712,7 +5124,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>900</v>
       </c>
@@ -5725,7 +5137,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -5735,7 +5147,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14">
+    <row r="23" spans="1:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -5745,7 +5157,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14">
+    <row r="24" spans="1:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -5755,7 +5167,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -5773,49 +5185,49 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0400-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0400-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0400-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0400-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0400-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0400-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0400-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0400-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0400-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0400-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
@@ -5823,45 +5235,45 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1"/>
+    <col min="3" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:14">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:14">
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -5880,8 +5292,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -5889,7 +5301,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:14">
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -5915,7 +5327,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" s="1" customFormat="1" spans="1:14">
+    <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -5939,7 +5351,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" s="1" customFormat="1" spans="1:14">
+    <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -5963,7 +5375,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:14">
+    <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -5987,7 +5399,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" s="1" customFormat="1" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>5</v>
       </c>
@@ -6005,7 +5417,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="1:14">
+    <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -6029,7 +5441,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -6039,7 +5451,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="1:14">
+    <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -6055,7 +5467,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:14">
+    <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -6071,7 +5483,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -6081,7 +5493,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:14">
+    <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -6097,7 +5509,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="1:14">
+    <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -6113,7 +5525,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="1:14">
+    <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -6129,7 +5541,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:14">
+    <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
@@ -6145,7 +5557,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" s="1" customFormat="1" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -6155,7 +5567,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" s="1" customFormat="1" spans="1:14">
+    <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -6171,7 +5583,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" s="1" customFormat="1" spans="1:14">
+    <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -6187,8 +5599,8 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" s="1" customFormat="1" spans="1:14">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:14">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -6203,8 +5615,8 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" s="1" customFormat="1" spans="1:14">
-      <c r="A21" s="2"/>
+    <row r="21" spans="1:14">
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>100</v>
       </c>
@@ -6217,7 +5629,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" s="1" customFormat="1" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -6227,7 +5639,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" s="1" customFormat="1" spans="1:14">
+    <row r="23" spans="1:14">
       <c r="A23"/>
       <c r="B23"/>
       <c r="D23" s="3"/>
@@ -6239,7 +5651,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" s="1" customFormat="1" spans="1:14">
+    <row r="24" spans="1:14">
       <c r="A24"/>
       <c r="B24"/>
       <c r="D24" s="3"/>
@@ -6251,7 +5663,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" s="1" customFormat="1" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -6269,49 +5681,49 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0500-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0500-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0500-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0500-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0500-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0500-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0500-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0500-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0500-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0500-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
@@ -6319,18 +5731,18 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.66666666666667" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="1"/>
+    <col min="3" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -6340,22 +5752,22 @@
       <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -6376,8 +5788,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -6483,7 +5895,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>5</v>
       </c>
@@ -6525,7 +5937,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -6567,7 +5979,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -6641,7 +6053,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -6684,7 +6096,7 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -6700,7 +6112,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>900</v>
       </c>
@@ -6713,7 +6125,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -6723,7 +6135,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14">
+    <row r="23" spans="1:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -6733,7 +6145,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14">
+    <row r="24" spans="1:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -6743,7 +6155,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -6761,49 +6173,49 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0600-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0600-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0600-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0600-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0600-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0600-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0600-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0600-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0600-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0600-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
@@ -6811,18 +6223,18 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33333333333333" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1"/>
+    <col min="3" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -6832,22 +6244,22 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -6868,8 +6280,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -6975,7 +6387,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>4</v>
       </c>
@@ -7017,7 +6429,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3">
         <v>2</v>
       </c>
@@ -7067,7 +6479,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -7141,7 +6553,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -7184,7 +6596,7 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -7200,7 +6612,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>1000</v>
       </c>
@@ -7213,7 +6625,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -7223,7 +6635,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14">
+    <row r="23" spans="1:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -7233,7 +6645,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14">
+    <row r="24" spans="1:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -7243,7 +6655,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -7261,49 +6673,49 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0700-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0700-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0700-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0700-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0700-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0700-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0700-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0700-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0700-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0700-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N25"/>
   <sheetViews>
@@ -7311,18 +6723,18 @@
       <selection activeCell="A19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.3333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33333333333333" style="1"/>
-    <col min="3" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="18.8333333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="13" width="11.3333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1"/>
+    <col min="3" max="8" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.16666666666667" style="1"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -7332,22 +6744,22 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -7368,8 +6780,8 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
@@ -7475,7 +6887,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:14">
+    <row r="7" spans="1:14">
       <c r="D7" s="3">
         <v>7</v>
       </c>
@@ -7517,7 +6929,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="1:14">
       <c r="D9" s="3">
         <v>4</v>
       </c>
@@ -7567,7 +6979,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="1:14">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -7641,7 +7053,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="4:14">
+    <row r="17" spans="1:14">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -7684,7 +7096,7 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="3">
@@ -7700,7 +7112,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3">
         <v>100</v>
       </c>
@@ -7713,7 +7125,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="4:14">
+    <row r="22" spans="1:14">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -7723,7 +7135,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="4:14">
+    <row r="23" spans="1:14">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -7733,7 +7145,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="4:14">
+    <row r="24" spans="1:14">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -7743,7 +7155,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="4:14">
+    <row r="25" spans="1:14">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -7761,43 +7173,43 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"全部,早爆,晚爆"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{00000000-0002-0000-0800-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>"前院,后院,屋顶"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"上炸下,下炸上,正炸"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25" xr:uid="{00000000-0002-0000-0800-000004000000}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0800-000005000000}">
       <formula1>"南瓜,普通,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0800-000006000000}">
       <formula1>"通常波,旗帜波"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0800-000007000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0800-000008000000}">
       <formula1>"卡,炮"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19" xr:uid="{00000000-0002-0000-0800-000009000000}">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25" xr:uid="{00000000-0002-0000-0800-00000A000000}">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25" xr:uid="{00000000-0002-0000-0800-00000B000000}">
       <formula1>"永动,非永动"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified:   Jack/batch_test/Jack_cpp_1_0.cpp 	modified:   Jack/jack_config.json 	modified:   Jack/jack_test_info.xlsx 	modified:   output.csv 	modified:   test.cpp
</commit_message>
<xml_diff>
--- a/Jack/jack_test_info.xlsx
+++ b/Jack/jack_test_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="21270" windowHeight="17775"/>
+    <workbookView windowWidth="24450" windowHeight="6405"/>
   </bookViews>
   <sheets>
     <sheet name="9" sheetId="5" r:id="rId1"/>
@@ -1354,7 +1354,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
@@ -1459,7 +1459,7 @@
         <v>161</v>
       </c>
       <c r="M3" s="6">
-        <v>440</v>
+        <v>550</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>20</v>
@@ -1620,7 +1620,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="3">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>

</xml_diff>

<commit_message>
modified:   Jack/batch_test/Jack_cpp_1_0.cpp 	new file:   Jack/batch_test/results.csv 	modified:   Jack/jack_config.json 	modified:   Jack/jack_test_info.xlsx 	modified:   "\347\275\256\344\277\241\345\214\272\351\227\264\344\270\216\345\201\207\350\256\276\346\243\200\351\252\214.ipynb"
</commit_message>
<xml_diff>
--- a/Jack/jack_test_info.xlsx
+++ b/Jack/jack_test_info.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="24450" windowHeight="6405"/>
+    <workbookView windowWidth="14040" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="9" sheetId="5" r:id="rId1"/>
-    <sheet name="6" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="16" r:id="rId3"/>
-    <sheet name="5" sheetId="4" r:id="rId4"/>
-    <sheet name="8列炮" sheetId="3" r:id="rId5"/>
+    <sheet name="8列炮" sheetId="3" r:id="rId2"/>
+    <sheet name="6" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId4"/>
+    <sheet name="5" sheetId="4" r:id="rId5"/>
     <sheet name="3" sheetId="10" r:id="rId6"/>
     <sheet name="7-N" sheetId="14" r:id="rId7"/>
     <sheet name="6-2" sheetId="1" r:id="rId8"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="45">
   <si>
     <t>小丑类型</t>
   </si>
@@ -104,9 +104,6 @@
     <t>非永动</t>
   </si>
   <si>
-    <t>卡</t>
-  </si>
-  <si>
     <t>被炸植物列数</t>
   </si>
   <si>
@@ -155,6 +152,15 @@
     <t>锁植物攻击间隔</t>
   </si>
   <si>
+    <t>最慢</t>
+  </si>
+  <si>
+    <t>正炸</t>
+  </si>
+  <si>
+    <t>炮</t>
+  </si>
+  <si>
     <t>全部</t>
   </si>
   <si>
@@ -162,12 +168,6 @@
   </si>
   <si>
     <t>上炸下</t>
-  </si>
-  <si>
-    <t>正炸</t>
-  </si>
-  <si>
-    <t>炮</t>
   </si>
   <si>
     <t>旗帜波</t>
@@ -1353,8 +1353,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
@@ -1452,28 +1452,22 @@
         <v>19</v>
       </c>
       <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>440</v>
+      </c>
       <c r="K3" s="3">
         <v>161</v>
       </c>
-      <c r="M3" s="6">
-        <v>550</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="6">
-        <v>447</v>
-      </c>
-      <c r="P3" s="6">
-        <v>719</v>
-      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>9</v>
@@ -1488,7 +1482,7 @@
         <v>19</v>
       </c>
       <c r="G4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="3"/>
       <c r="K4" s="3"/>
@@ -1499,10 +1493,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -1514,7 +1508,7 @@
         <v>19</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="3"/>
       <c r="K5" s="3"/>
@@ -1525,10 +1519,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -1537,7 +1531,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -1554,7 +1548,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>19</v>
@@ -1571,19 +1565,19 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D8" s="3">
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -1600,10 +1594,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -1617,10 +1611,10 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
-        <v>10000000</v>
+        <v>100000000</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1635,10 +1629,10 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1665,7 +1659,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -1683,7 +1677,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -1701,10 +1695,10 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1719,10 +1713,10 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -1923,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1983,7 +1977,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -1992,7 +1986,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -2005,7 +1999,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -2016,7 +2010,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>5</v>
@@ -2028,7 +2022,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -2042,10 +2036,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -2054,7 +2048,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -2068,10 +2062,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -2080,7 +2074,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -2097,10 +2091,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2114,7 +2108,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2123,10 +2117,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -2143,10 +2137,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -2160,7 +2154,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>1000000</v>
@@ -2178,10 +2172,10 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -2208,7 +2202,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -2226,7 +2220,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -2244,7 +2238,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>43</v>
@@ -2262,10 +2256,10 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -2466,7 +2460,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2548,7 +2542,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -2559,7 +2553,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>7</v>
@@ -2571,7 +2565,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -2585,10 +2579,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -2597,7 +2591,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -2611,10 +2605,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -2623,7 +2617,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -2640,7 +2634,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>19</v>
@@ -2657,7 +2651,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2666,10 +2660,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -2686,10 +2680,10 @@
         <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -2703,7 +2697,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -2721,10 +2715,10 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -2751,7 +2745,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -2769,7 +2763,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -2787,7 +2781,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>43</v>
@@ -2805,10 +2799,10 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -3091,7 +3085,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -3102,7 +3096,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>9</v>
@@ -3128,10 +3122,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -3154,7 +3148,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>42</v>
@@ -3166,7 +3160,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -3183,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>19</v>
@@ -3200,7 +3194,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -3209,10 +3203,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -3229,10 +3223,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -3246,7 +3240,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -3264,10 +3258,10 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -3294,7 +3288,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -3312,7 +3306,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -3330,7 +3324,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>43</v>
@@ -3348,10 +3342,10 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -3552,7 +3546,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -3634,7 +3628,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -3645,7 +3639,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>4</v>
@@ -3657,7 +3651,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -3671,10 +3665,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -3683,7 +3677,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -3697,10 +3691,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -3709,7 +3703,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -3726,10 +3720,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -3743,7 +3737,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -3752,10 +3746,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -3781,7 +3775,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>500000</v>
@@ -3799,10 +3793,10 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -3829,7 +3823,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -3847,7 +3841,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -3865,7 +3859,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>43</v>
@@ -3883,10 +3877,10 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -4156,7 +4150,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -4171,7 +4165,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -4182,7 +4176,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>8</v>
@@ -4194,7 +4188,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -4208,10 +4202,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -4220,7 +4214,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -4234,10 +4228,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>7</v>
@@ -4246,7 +4240,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -4263,10 +4257,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -4280,7 +4274,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -4289,10 +4283,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -4309,10 +4303,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -4326,7 +4320,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>50000</v>
@@ -4335,10 +4329,10 @@
         <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
@@ -4352,10 +4346,10 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -4382,7 +4376,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -4400,7 +4394,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -4418,7 +4412,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>43</v>
@@ -4436,10 +4430,10 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -4609,6 +4603,540 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet48"/>
+  <dimension ref="A1:P25"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="25.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.16666666666667" style="1"/>
+    <col min="4" max="6" width="8.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.16666666666667" style="1"/>
+    <col min="9" max="9" width="10" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.16666666666667" style="1"/>
+    <col min="11" max="11" width="15.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.16666666666667" style="1"/>
+    <col min="13" max="14" width="5.125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="10.875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.16666666666667" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="M3" s="6">
+        <v>1048</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="6">
+        <v>100</v>
+      </c>
+      <c r="P3" s="6">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1400</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+    </row>
+    <row r="17" spans="4:16">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+    </row>
+    <row r="18" spans="4:16">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+    </row>
+    <row r="19" spans="4:16">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+    </row>
+    <row r="20" spans="4:16">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+    </row>
+    <row r="21" spans="4:16">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+    </row>
+    <row r="22" spans="4:16">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+    </row>
+    <row r="23" spans="4:16">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+    </row>
+    <row r="24" spans="4:16">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+    </row>
+    <row r="25" spans="4:16">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+  </mergeCells>
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"全部,早爆,晚爆"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"前院,后院,屋顶"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"上炸下,下炸上,正炸"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"南瓜,普通,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"通常波,旗帜波"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B16">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N25">
+      <formula1>"卡,炮"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P25"/>
@@ -4640,7 +5168,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -4666,7 +5194,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -4700,7 +5228,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -4709,7 +5237,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -4725,7 +5253,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>6</v>
@@ -4737,7 +5265,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -4751,10 +5279,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -4763,7 +5291,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -4777,10 +5305,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -4789,7 +5317,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -4806,10 +5334,10 @@
         <v>3</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -4823,7 +5351,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>8</v>
@@ -4832,10 +5360,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -4861,7 +5389,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -4879,10 +5407,10 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -4909,7 +5437,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -4927,7 +5455,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -4945,10 +5473,10 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -4963,10 +5491,10 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -5135,7 +5663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P25"/>
@@ -5167,7 +5695,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5193,7 +5721,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -5227,7 +5755,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -5236,7 +5764,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -5252,7 +5780,7 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>6</v>
@@ -5264,7 +5792,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -5278,10 +5806,10 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -5290,7 +5818,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -5304,10 +5832,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -5316,7 +5844,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -5333,10 +5861,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -5350,7 +5878,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>5</v>
@@ -5359,10 +5887,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -5388,7 +5916,7 @@
     </row>
     <row r="10" s="1" customFormat="1" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -5406,10 +5934,10 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -5436,7 +5964,7 @@
     </row>
     <row r="13" s="1" customFormat="1" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -5454,7 +5982,7 @@
     </row>
     <row r="14" s="1" customFormat="1" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -5472,10 +6000,10 @@
     </row>
     <row r="15" s="1" customFormat="1" spans="1:16">
       <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -5490,10 +6018,10 @@
     </row>
     <row r="16" s="1" customFormat="1" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -5662,7 +6190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:P25"/>
@@ -5694,7 +6222,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5776,7 +6304,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -5787,7 +6315,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>6</v>
@@ -5799,7 +6327,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -5813,10 +6341,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -5825,7 +6353,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -5839,7 +6367,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>42</v>
@@ -5851,7 +6379,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -5868,10 +6396,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -5885,7 +6413,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -5894,10 +6422,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -5914,10 +6442,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -5931,7 +6459,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -5949,10 +6477,10 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -5979,7 +6507,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -5997,7 +6525,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -6015,7 +6543,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>43</v>
@@ -6033,544 +6561,10 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-    </row>
-    <row r="17" spans="4:16">
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-    </row>
-    <row r="18" spans="4:16">
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-    </row>
-    <row r="19" spans="4:16">
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-    </row>
-    <row r="20" spans="4:16">
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-    </row>
-    <row r="21" spans="4:16">
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-    </row>
-    <row r="22" spans="4:16">
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-    </row>
-    <row r="23" spans="4:16">
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-    </row>
-    <row r="24" spans="4:16">
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-    </row>
-    <row r="25" spans="4:16">
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"全部,早爆,晚爆"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"前院,后院,屋顶"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"上炸下,下炸上,正炸"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"南瓜,普通,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"通常波,旗帜波"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B16">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N25">
-      <formula1>"卡,炮"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet48"/>
-  <dimension ref="A1:P25"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="25.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.16666666666667" style="1"/>
-    <col min="4" max="6" width="8.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.16666666666667" style="1"/>
-    <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.16666666666667" style="1"/>
-    <col min="11" max="11" width="15.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.16666666666667" style="1"/>
-    <col min="13" max="14" width="5.125" style="1" customWidth="1"/>
-    <col min="15" max="16" width="10.875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.16666666666667" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="3">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="M3" s="6">
-        <v>1039</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" s="6">
-        <v>100</v>
-      </c>
-      <c r="P3" s="6">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="3">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="D7" s="3">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="3">
-        <v>100000000</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1400</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -6771,7 +6765,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -6797,7 +6791,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -6831,7 +6825,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -6853,7 +6847,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -6864,7 +6858,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -6876,7 +6870,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -6893,10 +6887,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -6905,7 +6899,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -6919,10 +6913,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -6931,7 +6925,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -6948,10 +6942,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -6965,7 +6959,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -6974,10 +6968,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -7003,7 +6997,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -7021,10 +7015,10 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -7051,7 +7045,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -7069,7 +7063,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -7087,7 +7081,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>43</v>
@@ -7105,10 +7099,10 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -7309,7 +7303,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -7335,7 +7329,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -7378,7 +7372,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -7393,7 +7387,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -7404,7 +7398,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>7</v>
@@ -7416,7 +7410,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -7430,10 +7424,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -7442,7 +7436,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -7456,10 +7450,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -7468,7 +7462,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -7485,10 +7479,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -7502,7 +7496,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -7511,10 +7505,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -7540,7 +7534,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -7558,10 +7552,10 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -7588,7 +7582,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -7606,7 +7600,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -7624,7 +7618,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>43</v>
@@ -7642,10 +7636,10 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -7928,7 +7922,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -7939,7 +7933,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>6</v>
@@ -7951,7 +7945,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -7965,10 +7959,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -7977,7 +7971,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -7991,10 +7985,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -8003,7 +7997,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -8020,10 +8014,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -8037,7 +8031,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -8046,10 +8040,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -8075,7 +8069,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>100000000</v>
@@ -8093,10 +8087,10 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -8123,7 +8117,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -8141,7 +8135,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -8159,7 +8153,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>43</v>
@@ -8177,10 +8171,10 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -8441,7 +8435,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
@@ -8450,7 +8444,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -8463,7 +8457,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -8474,7 +8468,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>7</v>
@@ -8486,7 +8480,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -8500,10 +8494,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -8512,7 +8506,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -8526,10 +8520,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -8538,7 +8532,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -8555,10 +8549,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -8572,7 +8566,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -8581,10 +8575,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -8610,7 +8604,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>10000000</v>
@@ -8628,10 +8622,10 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -8658,7 +8652,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -8676,7 +8670,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>1400</v>
@@ -8694,7 +8688,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>43</v>
@@ -8712,10 +8706,10 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>

</xml_diff>

<commit_message>
七列樱桃 	modified:   Jack/jack_config.json 	modified:   Jack/jack_test_info.xlsx
</commit_message>
<xml_diff>
--- a/Jack/jack_test_info.xlsx
+++ b/Jack/jack_test_info.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="19830" windowHeight="17775"/>
+    <workbookView windowWidth="17325" windowHeight="7155"/>
   </bookViews>
   <sheets>
-    <sheet name="7" sheetId="13" r:id="rId1"/>
-    <sheet name="9" sheetId="5" r:id="rId2"/>
+    <sheet name="9" sheetId="5" r:id="rId1"/>
+    <sheet name="7" sheetId="13" r:id="rId2"/>
     <sheet name="8列炮" sheetId="3" r:id="rId3"/>
     <sheet name="6" sheetId="6" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="16" r:id="rId5"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="45">
   <si>
     <t>小丑类型</t>
   </si>
@@ -95,7 +95,7 @@
     <t>被炸情况</t>
   </si>
   <si>
-    <t>正炸</t>
+    <t>下炸上</t>
   </si>
   <si>
     <t>曾</t>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>被炸植物列数</t>
-  </si>
-  <si>
-    <t>永动</t>
   </si>
   <si>
     <t>被炸植物类型</t>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>冰瓜额外溅射次数</t>
+  </si>
+  <si>
+    <t>永动</t>
   </si>
   <si>
     <t>测试次数</t>
@@ -155,10 +155,7 @@
     <t>锁植物攻击间隔</t>
   </si>
   <si>
-    <t>下炸上</t>
-  </si>
-  <si>
-    <t>最慢</t>
+    <t>正炸</t>
   </si>
   <si>
     <t>炮</t>
@@ -1353,11 +1350,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet3"/>
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
@@ -1455,23 +1452,21 @@
         <v>19</v>
       </c>
       <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
         <v>1</v>
       </c>
+      <c r="I3" s="3"/>
       <c r="K3" s="3"/>
       <c r="M3" s="6">
-        <v>1069</v>
+        <v>600</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="O3" s="6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="P3" s="6">
-        <v>900</v>
+        <v>639</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1479,19 +1474,19 @@
         <v>21</v>
       </c>
       <c r="B4" s="3">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3">
         <v>8</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="3"/>
       <c r="K4" s="3"/>
@@ -1502,10 +1497,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -1514,10 +1509,10 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="3"/>
       <c r="K5" s="3"/>
@@ -1528,10 +1523,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -1540,10 +1535,10 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" s="3"/>
       <c r="K6" s="3"/>
@@ -1552,12 +1547,12 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>19</v>
@@ -1574,7 +1569,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -1583,10 +1578,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -1598,15 +1593,15 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -1654,7 +1649,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1671,7 +1666,7 @@
         <v>32</v>
       </c>
       <c r="B13" s="3">
-        <v>1044</v>
+        <v>0</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1952,7 +1947,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -1986,7 +1981,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
@@ -1995,7 +1990,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -2008,7 +2003,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -2031,7 +2026,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -2045,10 +2040,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -2057,7 +2052,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -2071,10 +2066,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -2083,7 +2078,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -2095,15 +2090,15 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2117,7 +2112,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2126,10 +2121,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -2141,7 +2136,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -2189,7 +2184,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -2242,7 +2237,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2461,7 +2456,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2521,7 +2516,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -2530,7 +2525,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -2543,7 +2538,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -2566,7 +2561,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -2580,10 +2575,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -2592,7 +2587,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -2606,10 +2601,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -2618,7 +2613,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -2630,15 +2625,15 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2652,7 +2647,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2661,10 +2656,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -2676,15 +2671,15 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3">
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -2732,7 +2727,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -2785,7 +2780,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3064,7 +3059,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3">
         <v>9</v>
@@ -3086,7 +3081,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -3123,10 +3118,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -3149,10 +3144,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -3161,7 +3156,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -3173,12 +3168,12 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>19</v>
@@ -3195,7 +3190,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -3204,10 +3199,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -3219,15 +3214,15 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3">
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -3275,7 +3270,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -3328,7 +3323,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3547,7 +3542,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -3607,7 +3602,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -3629,7 +3624,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -3652,7 +3647,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -3666,10 +3661,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -3678,7 +3673,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -3692,10 +3687,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -3704,7 +3699,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -3716,15 +3711,15 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -3738,7 +3733,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -3747,10 +3742,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -3762,7 +3757,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -3810,7 +3805,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -3863,7 +3858,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -4142,7 +4137,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3">
         <v>5</v>
@@ -4151,7 +4146,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -4166,7 +4161,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -4189,7 +4184,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -4203,10 +4198,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -4215,7 +4210,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -4229,10 +4224,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>7</v>
@@ -4241,7 +4236,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -4253,15 +4248,15 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -4275,7 +4270,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -4284,10 +4279,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -4299,15 +4294,15 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3">
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -4330,10 +4325,10 @@
         <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
@@ -4363,7 +4358,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -4416,7 +4411,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -4605,11 +4600,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet7"/>
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.5"/>
@@ -4707,37 +4702,43 @@
         <v>19</v>
       </c>
       <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
         <v>1</v>
       </c>
-      <c r="I3" s="3">
-        <v>440</v>
-      </c>
-      <c r="K3" s="3">
-        <v>161</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="K3" s="3"/>
+      <c r="M3" s="6">
+        <v>1069</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="6">
+        <v>100</v>
+      </c>
+      <c r="P3" s="6">
+        <v>900</v>
+      </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3"/>
       <c r="K4" s="3"/>
@@ -4748,10 +4749,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -4760,10 +4761,10 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="3"/>
       <c r="K5" s="3"/>
@@ -4774,10 +4775,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -4786,7 +4787,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -4798,12 +4799,12 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>19</v>
@@ -4820,19 +4821,19 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8" s="3">
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -4844,15 +4845,15 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -4869,7 +4870,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="3">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -4900,7 +4901,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -4917,7 +4918,7 @@
         <v>32</v>
       </c>
       <c r="B13" s="3">
-        <v>0</v>
+        <v>1044</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -4971,7 +4972,7 @@
         <v>36</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -5231,7 +5232,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
@@ -5240,7 +5241,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -5253,7 +5254,7 @@
         <v>1048</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -5276,7 +5277,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -5290,10 +5291,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -5302,7 +5303,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -5316,10 +5317,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -5328,7 +5329,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -5340,15 +5341,15 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -5362,7 +5363,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -5371,10 +5372,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -5386,7 +5387,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -5434,7 +5435,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -5706,7 +5707,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5732,7 +5733,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -5766,7 +5767,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -5775,7 +5776,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -5803,7 +5804,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -5817,10 +5818,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -5829,7 +5830,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -5843,10 +5844,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -5855,7 +5856,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -5867,15 +5868,15 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>3</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -5889,7 +5890,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>8</v>
@@ -5898,10 +5899,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -5913,7 +5914,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -5961,7 +5962,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -6233,7 +6234,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -6259,7 +6260,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -6293,7 +6294,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -6302,7 +6303,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -6330,7 +6331,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -6344,10 +6345,10 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -6356,7 +6357,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -6370,10 +6371,10 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -6382,7 +6383,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -6394,15 +6395,15 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:16">
+    <row r="7" s="1" customFormat="1" spans="4:16">
       <c r="D7" s="3">
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -6416,7 +6417,7 @@
     </row>
     <row r="8" s="1" customFormat="1" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>5</v>
@@ -6425,10 +6426,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -6440,7 +6441,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="1:16">
+    <row r="9" s="1" customFormat="1" spans="4:16">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -6488,7 +6489,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:16">
+    <row r="12" s="1" customFormat="1" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -6760,7 +6761,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -6820,7 +6821,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -6842,7 +6843,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -6865,7 +6866,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -6879,10 +6880,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -6891,7 +6892,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -6905,10 +6906,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -6917,7 +6918,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -6929,15 +6930,15 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -6951,7 +6952,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -6960,10 +6961,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -6975,15 +6976,15 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3">
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -7031,7 +7032,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -7084,7 +7085,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -7303,7 +7304,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -7329,7 +7330,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -7363,7 +7364,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -7385,7 +7386,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -7408,7 +7409,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -7425,10 +7426,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -7437,7 +7438,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -7451,10 +7452,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -7463,7 +7464,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -7475,15 +7476,15 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -7497,7 +7498,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -7506,10 +7507,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -7521,7 +7522,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -7569,7 +7570,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -7622,7 +7623,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -7841,7 +7842,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -7867,7 +7868,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -7901,7 +7902,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
@@ -7910,7 +7911,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -7925,7 +7926,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -7948,7 +7949,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -7962,10 +7963,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -7974,7 +7975,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -7988,10 +7989,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -8000,7 +8001,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -8012,15 +8013,15 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -8034,7 +8035,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -8043,10 +8044,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -8058,7 +8059,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -8106,7 +8107,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -8159,7 +8160,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -8438,7 +8439,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3">
         <v>6</v>
@@ -8460,7 +8461,7 @@
         <v>1039</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="6">
         <v>100</v>
@@ -8483,7 +8484,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -8497,10 +8498,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -8509,7 +8510,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -8523,10 +8524,10 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -8535,7 +8536,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -8547,15 +8548,15 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="4:16">
       <c r="D7" s="3">
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -8569,7 +8570,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -8578,10 +8579,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -8593,7 +8594,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="4:16">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -8641,7 +8642,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="4:16">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -8694,7 +8695,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>

</xml_diff>